<commit_message>
Change random test for memory
</commit_message>
<xml_diff>
--- a/pendulum/random_full_grav/random_full_raw_data.xlsx
+++ b/pendulum/random_full_grav/random_full_raw_data.xlsx
@@ -493,7 +493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -593,6 +593,16 @@
         <v>-67</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>conditional(add(add(x, vel), add(add(x, x), conditional(x, x))), add(add(add(x, y), add(vel, x)), add(add(x, y), y)))</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>-419</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>